<commit_message>
updated squash for R25 and R50
</commit_message>
<xml_diff>
--- a/Results/Profit TAV Manuscript R50.xlsx
+++ b/Results/Profit TAV Manuscript R50.xlsx
@@ -1,104 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tigermailauburn-my.sharepoint.com/personal/bzm0094_auburn_edu/Documents/Collaboration/Ngbede M/Agrivoltaics-alabama/Results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_FF4CE279035F68FDDF6BD283E1D95554392D33A5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDD514E9-D23F-4972-AFA1-BFD08C8FBF7C}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" firstSheet="0" windowHeight="13125" windowWidth="13125" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Row_Names</t>
-  </si>
-  <si>
-    <t>04.6</t>
-  </si>
-  <si>
-    <t>06.4</t>
-  </si>
-  <si>
-    <t>08.2</t>
-  </si>
-  <si>
-    <t>0.254.6</t>
-  </si>
-  <si>
-    <t>0.256.4</t>
-  </si>
-  <si>
-    <t>0.258.2</t>
-  </si>
-  <si>
-    <t>0.54.6</t>
-  </si>
-  <si>
-    <t>0.56.4</t>
-  </si>
-  <si>
-    <t>0.58.2</t>
-  </si>
-  <si>
-    <t>0.754.6</t>
-  </si>
-  <si>
-    <t>0.756.4</t>
-  </si>
-  <si>
-    <t>0.758.2</t>
-  </si>
-  <si>
-    <t>14.6</t>
-  </si>
-  <si>
-    <t>16.4</t>
-  </si>
-  <si>
-    <t>18.2</t>
-  </si>
-  <si>
-    <t>0.04201NorthernFixed</t>
-  </si>
-  <si>
-    <t>0.04201CentralFixed</t>
-  </si>
-  <si>
-    <t>0.04201Black BeltFixed</t>
-  </si>
-  <si>
-    <t>0.04201SouthernFixed</t>
-  </si>
-  <si>
-    <t>0.04201NorthernTracking</t>
-  </si>
-  <si>
-    <t>0.04201CentralTracking</t>
-  </si>
-  <si>
-    <t>0.04201Black BeltTracking</t>
-  </si>
-  <si>
-    <t>0.04201SouthernTracking</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,38 +49,29 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P9" totalsRowShown="0">
-  <autoFilter ref="A1:P9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" id="1" name="Table1" displayName="Table1" ref="A1:P9" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Row_Names"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="04.6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="06.4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="08.2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="0.254.6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="0.256.4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="0.258.2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="0.54.6"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="0.56.4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="0.58.2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="0.754.6"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="0.756.4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="0.758.2"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="14.6"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="16.4"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="18.2"/>
+    <tableColumn id="1" name="Row_Names"/>
+    <tableColumn id="2" name="04.6"/>
+    <tableColumn id="3" name="06.4"/>
+    <tableColumn id="4" name="08.2"/>
+    <tableColumn id="5" name="0.254.6"/>
+    <tableColumn id="6" name="0.256.4"/>
+    <tableColumn id="7" name="0.258.2"/>
+    <tableColumn id="8" name="0.54.6"/>
+    <tableColumn id="9" name="0.56.4"/>
+    <tableColumn id="10" name="0.58.2"/>
+    <tableColumn id="11" name="0.754.6"/>
+    <tableColumn id="12" name="0.756.4"/>
+    <tableColumn id="13" name="0.758.2"/>
+    <tableColumn id="14" name="14.6"/>
+    <tableColumn id="15" name="16.4"/>
+    <tableColumn id="16" name="18.2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -487,76 +393,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="1" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Row_Names</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>04.6</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>06.4</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>08.2</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>0.254.6</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>0.256.4</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>0.258.2</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>0.54.6</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>0.56.4</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>0.58.2</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>0.754.6</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>0.756.4</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>0.758.2</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>14.6</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>16.4</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>18.2</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0.04201NorthernFixed</t>
+        </is>
       </c>
       <c r="B2">
         <v>9619</v>
@@ -604,9 +534,11 @@
         <v>13690</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0.04201CentralFixed</t>
+        </is>
       </c>
       <c r="B3">
         <v>9619</v>
@@ -654,9 +586,11 @@
         <v>14659</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0.04201Black BeltFixed</t>
+        </is>
       </c>
       <c r="B4">
         <v>9619</v>
@@ -704,9 +638,11 @@
         <v>15292</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0.04201SouthernFixed</t>
+        </is>
       </c>
       <c r="B5">
         <v>9619</v>
@@ -754,9 +690,11 @@
         <v>15522</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>0.04201NorthernTracking</t>
+        </is>
       </c>
       <c r="B6">
         <v>9619</v>
@@ -804,9 +742,11 @@
         <v>19693</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>0.04201CentralTracking</t>
+        </is>
       </c>
       <c r="B7">
         <v>9619</v>
@@ -854,9 +794,11 @@
         <v>21144</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0.04201Black BeltTracking</t>
+        </is>
       </c>
       <c r="B8">
         <v>9619</v>
@@ -904,9 +846,11 @@
         <v>21860</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>0.04201SouthernTracking</t>
+        </is>
       </c>
       <c r="B9">
         <v>9619</v>
@@ -955,7 +899,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="1"/>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">

</xml_diff>